<commit_message>
seems to be working with health system now
</commit_message>
<xml_diff>
--- a/resources/Method_Oesophageal_Cancer.xlsx
+++ b/resources/Method_Oesophageal_Cancer.xlsx
@@ -783,7 +783,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -871,7 +871,7 @@
         <xdr:cNvPr id="43" name="Oval 42">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00002B000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00002B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1040,7 +1040,7 @@
         <xdr:cNvPr id="44" name="TextBox 140">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00002C000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00002C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1196,7 +1196,7 @@
         <xdr:cNvPr id="45" name="Straight Arrow Connector 44">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00002D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00002D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1255,7 +1255,7 @@
         <xdr:cNvPr id="46" name="Rectangle 45">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00002E000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00002E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1397,7 +1397,7 @@
         <xdr:cNvPr id="47" name="Oval 46">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00002F000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00002F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1566,7 +1566,7 @@
         <xdr:cNvPr id="48" name="TextBox 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000030000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000030000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1710,7 +1710,7 @@
         <xdr:cNvPr id="49" name="TextBox 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000031000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000031000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1854,7 +1854,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1898,7 +1898,7 @@
         <xdr:cNvPr id="90" name="Picture 89">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00005A000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00005A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1948,7 +1948,7 @@
         <xdr:cNvPr id="97" name="Picture 96">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000061000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000061000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2003,7 +2003,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2064,7 +2064,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2125,7 +2125,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2186,7 +2186,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2247,7 +2247,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2308,7 +2308,7 @@
         <xdr:cNvPr id="8" name="Picture 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000008000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3431,7 +3431,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>